<commit_message>
Solución a taller de modulo R
</commit_message>
<xml_diff>
--- a/_modulo-R/talleres/ejemplo2.xlsx
+++ b/_modulo-R/talleres/ejemplo2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ejemplo2" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,11 +62,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +88,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,12 +137,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,12 +178,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -175,7 +193,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -189,7 +207,7 @@
       <c r="B2" s="0" t="n">
         <v>-1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -203,7 +221,7 @@
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -217,7 +235,7 @@
       <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -231,7 +249,7 @@
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -242,10 +260,10 @@
       <c r="A6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -258,6 +276,9 @@
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>11</v>

</xml_diff>